<commit_message>
Final change in check list
</commit_message>
<xml_diff>
--- a/Check-List.xlsx
+++ b/Check-List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MEDION\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MEDION\Desktop\Andruskevic_13march2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A80D86-2702-4C68-B8F6-40631331257C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2580AA0F-E729-49E8-A3D3-5E66319BDF84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Browsers</t>
   </si>
@@ -84,67 +84,7 @@
     <t>"Не нашли что искали?" message and form field  are displayed if no product matches the search</t>
   </si>
   <si>
-    <t>Cart</t>
-  </si>
-  <si>
     <t>Non cyrillic alphabet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add product to cart </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product is added to the cart </t>
-  </si>
-  <si>
-    <t>Cart visibility after adding product</t>
-  </si>
-  <si>
-    <t>The product appears in the cart after being added</t>
-  </si>
-  <si>
-    <t>Delete product from the cart</t>
-  </si>
-  <si>
-    <t>Product is deleted from the cart</t>
-  </si>
-  <si>
-    <t>Cart contents after page refresh</t>
-  </si>
-  <si>
-    <t>Items remain in the cart after refreshing the page</t>
-  </si>
-  <si>
-    <t>Authorization</t>
-  </si>
-  <si>
-    <t>Display and functionality of the authorization form</t>
-  </si>
-  <si>
-    <t>The authorization form is displayed correctly with fields for country, phone, and email</t>
-  </si>
-  <si>
-    <t>Validation for empty fields</t>
-  </si>
-  <si>
-    <t>Appear error message "Please fill out this field"</t>
-  </si>
-  <si>
-    <t>Validation of the email field for correct format</t>
-  </si>
-  <si>
-    <t>Appear error message where symbol "@" is require</t>
-  </si>
-  <si>
-    <t>Validation of the phone field for correct format</t>
-  </si>
-  <si>
-    <t>Appear error message where phone format is incorrect</t>
-  </si>
-  <si>
-    <t>Country list dropdown functionality</t>
-  </si>
-  <si>
-    <t>The country list dropdown works properly and allows for easy selection</t>
   </si>
   <si>
     <t>UI</t>
@@ -160,20 +100,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="186"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -393,40 +325,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -435,29 +355,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
@@ -757,21 +677,21 @@
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -780,281 +700,133 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="8">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="8">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="8">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="8">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>6</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
         <v>16</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
-        <v>7</v>
-      </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <v>8</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
-        <v>9</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
-    </row>
-    <row r="14" spans="1:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>10</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
-        <v>11</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
-        <v>12</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
-        <v>13</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
-        <v>14</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
-        <v>15</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
-        <v>16</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A21:F21"/>
+  <mergeCells count="3">
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>